<commit_message>
added all repo list
</commit_message>
<xml_diff>
--- a/cli/LP Github repos.xlsx
+++ b/cli/LP Github repos.xlsx
@@ -436,7 +436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1116,6 +1116,216 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>xAI-Console-UI</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Yes (NPM)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>xAI-Inference-server</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Yes (NPM)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>xAI-Labelling-UI</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Yes (NPM and Yarn)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>xapi-js-client</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Yes (NPM)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Renovate and Dependabot</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>yum-api-qatests</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Yes (NPM)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>